<commit_message>
added names of polling stations T2 2024
</commit_message>
<xml_diff>
--- a/raw_data/legislatives2024_t2_9213.xlsx
+++ b/raw_data/legislatives2024_t2_9213.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BD93"/>
+  <dimension ref="A1:BF93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -707,6 +707,16 @@
       <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>Elu 4</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>id_bv2</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>nomBureauVote</t>
         </is>
       </c>
     </row>
@@ -893,6 +903,16 @@
       <c r="BB2" t="inlineStr"/>
       <c r="BC2" t="inlineStr"/>
       <c r="BD2" t="inlineStr"/>
+      <c r="BE2" t="inlineStr">
+        <is>
+          <t>92002_1</t>
+        </is>
+      </c>
+      <c r="BF2" t="inlineStr">
+        <is>
+          <t>001 HOTEL DE VILLE SALLE DU CONSEIL</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -1077,6 +1097,16 @@
       <c r="BB3" t="inlineStr"/>
       <c r="BC3" t="inlineStr"/>
       <c r="BD3" t="inlineStr"/>
+      <c r="BE3" t="inlineStr">
+        <is>
+          <t>92002_2</t>
+        </is>
+      </c>
+      <c r="BF3" t="inlineStr">
+        <is>
+          <t>002 ECOLE ELEM F BUISSON PREAU</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -1261,6 +1291,16 @@
       <c r="BB4" t="inlineStr"/>
       <c r="BC4" t="inlineStr"/>
       <c r="BD4" t="inlineStr"/>
+      <c r="BE4" t="inlineStr">
+        <is>
+          <t>92002_3</t>
+        </is>
+      </c>
+      <c r="BF4" t="inlineStr">
+        <is>
+          <t>003 ECOLE ELEM VELPEAU REFECTOIRE</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -1445,6 +1485,16 @@
       <c r="BB5" t="inlineStr"/>
       <c r="BC5" t="inlineStr"/>
       <c r="BD5" t="inlineStr"/>
+      <c r="BE5" t="inlineStr">
+        <is>
+          <t>92002_4</t>
+        </is>
+      </c>
+      <c r="BF5" t="inlineStr">
+        <is>
+          <t>004 ECOLE MATER VELPEAU SALLE DE JEUX</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -1629,6 +1679,16 @@
       <c r="BB6" t="inlineStr"/>
       <c r="BC6" t="inlineStr"/>
       <c r="BD6" t="inlineStr"/>
+      <c r="BE6" t="inlineStr">
+        <is>
+          <t>92002_5</t>
+        </is>
+      </c>
+      <c r="BF6" t="inlineStr">
+        <is>
+          <t>005 ECOLE MATER VELPEAU REFECTOIRE</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -1813,6 +1873,16 @@
       <c r="BB7" t="inlineStr"/>
       <c r="BC7" t="inlineStr"/>
       <c r="BD7" t="inlineStr"/>
+      <c r="BE7" t="inlineStr">
+        <is>
+          <t>92002_6</t>
+        </is>
+      </c>
+      <c r="BF7" t="inlineStr">
+        <is>
+          <t>006 MAISON DES ANS TONIQUES</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -1997,6 +2067,16 @@
       <c r="BB8" t="inlineStr"/>
       <c r="BC8" t="inlineStr"/>
       <c r="BD8" t="inlineStr"/>
+      <c r="BE8" t="inlineStr">
+        <is>
+          <t>92002_7</t>
+        </is>
+      </c>
+      <c r="BF8" t="inlineStr">
+        <is>
+          <t>007 ECOLE MATERNELLE JEAN MOULIN</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -2181,6 +2261,16 @@
       <c r="BB9" t="inlineStr"/>
       <c r="BC9" t="inlineStr"/>
       <c r="BD9" t="inlineStr"/>
+      <c r="BE9" t="inlineStr">
+        <is>
+          <t>92002_8</t>
+        </is>
+      </c>
+      <c r="BF9" t="inlineStr">
+        <is>
+          <t>008 ECOLE MATERNELLE LA FONTAINE PREAU</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -2365,6 +2455,16 @@
       <c r="BB10" t="inlineStr"/>
       <c r="BC10" t="inlineStr"/>
       <c r="BD10" t="inlineStr"/>
+      <c r="BE10" t="inlineStr">
+        <is>
+          <t>92002_9</t>
+        </is>
+      </c>
+      <c r="BF10" t="inlineStr">
+        <is>
+          <t>009 ECOLE ELEM LA FONTAINE REFECTOIRE</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -2549,6 +2649,16 @@
       <c r="BB11" t="inlineStr"/>
       <c r="BC11" t="inlineStr"/>
       <c r="BD11" t="inlineStr"/>
+      <c r="BE11" t="inlineStr">
+        <is>
+          <t>92002_10</t>
+        </is>
+      </c>
+      <c r="BF11" t="inlineStr">
+        <is>
+          <t>010 ECOLE MATERNELLE ANDRE PASQUIER</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -2733,6 +2843,16 @@
       <c r="BB12" t="inlineStr"/>
       <c r="BC12" t="inlineStr"/>
       <c r="BD12" t="inlineStr"/>
+      <c r="BE12" t="inlineStr">
+        <is>
+          <t>92002_11</t>
+        </is>
+      </c>
+      <c r="BF12" t="inlineStr">
+        <is>
+          <t>011 ECOLE MATER F BUISSON PREAU</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -2917,6 +3037,16 @@
       <c r="BB13" t="inlineStr"/>
       <c r="BC13" t="inlineStr"/>
       <c r="BD13" t="inlineStr"/>
+      <c r="BE13" t="inlineStr">
+        <is>
+          <t>92002_12</t>
+        </is>
+      </c>
+      <c r="BF13" t="inlineStr">
+        <is>
+          <t>012 ECOLE ELEM F BUISSON BIBLIOTHEQ</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -3101,6 +3231,16 @@
       <c r="BB14" t="inlineStr"/>
       <c r="BC14" t="inlineStr"/>
       <c r="BD14" t="inlineStr"/>
+      <c r="BE14" t="inlineStr">
+        <is>
+          <t>92002_13</t>
+        </is>
+      </c>
+      <c r="BF14" t="inlineStr">
+        <is>
+          <t>013 HOTEL DE VILLE SALON D HONNEUR</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -3285,6 +3425,16 @@
       <c r="BB15" t="inlineStr"/>
       <c r="BC15" t="inlineStr"/>
       <c r="BD15" t="inlineStr"/>
+      <c r="BE15" t="inlineStr">
+        <is>
+          <t>92002_14</t>
+        </is>
+      </c>
+      <c r="BF15" t="inlineStr">
+        <is>
+          <t>014 ECOLE ELEMENTAIRE J FERRY PREAU</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -3469,6 +3619,16 @@
       <c r="BB16" t="inlineStr"/>
       <c r="BC16" t="inlineStr"/>
       <c r="BD16" t="inlineStr"/>
+      <c r="BE16" t="inlineStr">
+        <is>
+          <t>92002_15</t>
+        </is>
+      </c>
+      <c r="BF16" t="inlineStr">
+        <is>
+          <t>015 ECOLE ELEM J FERRY REFECTOIRE</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -3653,6 +3813,16 @@
       <c r="BB17" t="inlineStr"/>
       <c r="BC17" t="inlineStr"/>
       <c r="BD17" t="inlineStr"/>
+      <c r="BE17" t="inlineStr">
+        <is>
+          <t>92002_16</t>
+        </is>
+      </c>
+      <c r="BF17" t="inlineStr">
+        <is>
+          <t>016 ECOLE MATERNELLE J FERRY PREAU</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -3837,6 +4007,16 @@
       <c r="BB18" t="inlineStr"/>
       <c r="BC18" t="inlineStr"/>
       <c r="BD18" t="inlineStr"/>
+      <c r="BE18" t="inlineStr">
+        <is>
+          <t>92002_17</t>
+        </is>
+      </c>
+      <c r="BF18" t="inlineStr">
+        <is>
+          <t>017 ECOLE ELEM E BLANGUERNON PREAU</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -4021,6 +4201,16 @@
       <c r="BB19" t="inlineStr"/>
       <c r="BC19" t="inlineStr"/>
       <c r="BD19" t="inlineStr"/>
+      <c r="BE19" t="inlineStr">
+        <is>
+          <t>92002_18</t>
+        </is>
+      </c>
+      <c r="BF19" t="inlineStr">
+        <is>
+          <t>018 ECOLE ELEM E BLANGUERNON REFECT</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -4205,6 +4395,16 @@
       <c r="BB20" t="inlineStr"/>
       <c r="BC20" t="inlineStr"/>
       <c r="BD20" t="inlineStr"/>
+      <c r="BE20" t="inlineStr">
+        <is>
+          <t>92002_19</t>
+        </is>
+      </c>
+      <c r="BF20" t="inlineStr">
+        <is>
+          <t>019 ECOLE MATERNELLE ANDRE CHENIER</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -4389,6 +4589,16 @@
       <c r="BB21" t="inlineStr"/>
       <c r="BC21" t="inlineStr"/>
       <c r="BD21" t="inlineStr"/>
+      <c r="BE21" t="inlineStr">
+        <is>
+          <t>92002_20</t>
+        </is>
+      </c>
+      <c r="BF21" t="inlineStr">
+        <is>
+          <t>020 ECOLE ELEM E BLANGUERNON PREAU</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -4573,6 +4783,16 @@
       <c r="BB22" t="inlineStr"/>
       <c r="BC22" t="inlineStr"/>
       <c r="BD22" t="inlineStr"/>
+      <c r="BE22" t="inlineStr">
+        <is>
+          <t>92002_21</t>
+        </is>
+      </c>
+      <c r="BF22" t="inlineStr">
+        <is>
+          <t>021 CENTRE DE LOISIRS DU PARC HELLER</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -4757,6 +4977,16 @@
       <c r="BB23" t="inlineStr"/>
       <c r="BC23" t="inlineStr"/>
       <c r="BD23" t="inlineStr"/>
+      <c r="BE23" t="inlineStr">
+        <is>
+          <t>92002_22</t>
+        </is>
+      </c>
+      <c r="BF23" t="inlineStr">
+        <is>
+          <t>022 CENTRE DE LOISIRS DU PARC HELLER</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -4941,6 +5171,16 @@
       <c r="BB24" t="inlineStr"/>
       <c r="BC24" t="inlineStr"/>
       <c r="BD24" t="inlineStr"/>
+      <c r="BE24" t="inlineStr">
+        <is>
+          <t>92002_23</t>
+        </is>
+      </c>
+      <c r="BF24" t="inlineStr">
+        <is>
+          <t>023 ECOLE MATERNELLE PAUL BERT PREAU</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -5125,6 +5365,16 @@
       <c r="BB25" t="inlineStr"/>
       <c r="BC25" t="inlineStr"/>
       <c r="BD25" t="inlineStr"/>
+      <c r="BE25" t="inlineStr">
+        <is>
+          <t>92002_24</t>
+        </is>
+      </c>
+      <c r="BF25" t="inlineStr">
+        <is>
+          <t>024 ECOLE MAT PAUL BERT REFECTOIRE</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -5309,6 +5559,16 @@
       <c r="BB26" t="inlineStr"/>
       <c r="BC26" t="inlineStr"/>
       <c r="BD26" t="inlineStr"/>
+      <c r="BE26" t="inlineStr">
+        <is>
+          <t>92002_25</t>
+        </is>
+      </c>
+      <c r="BF26" t="inlineStr">
+        <is>
+          <t>025 ECOLE ELEMENTAIRE PAUL BERT PREAU</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -5493,6 +5753,16 @@
       <c r="BB27" t="inlineStr"/>
       <c r="BC27" t="inlineStr"/>
       <c r="BD27" t="inlineStr"/>
+      <c r="BE27" t="inlineStr">
+        <is>
+          <t>92002_26</t>
+        </is>
+      </c>
+      <c r="BF27" t="inlineStr">
+        <is>
+          <t>026 ECOLE MAT A PAJEAUD SALLE DE JEUX</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -5677,6 +5947,16 @@
       <c r="BB28" t="inlineStr"/>
       <c r="BC28" t="inlineStr"/>
       <c r="BD28" t="inlineStr"/>
+      <c r="BE28" t="inlineStr">
+        <is>
+          <t>92002_27</t>
+        </is>
+      </c>
+      <c r="BF28" t="inlineStr">
+        <is>
+          <t>027 ECOLE ELEM A PAJEAUD REFECTOIRE</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -5861,6 +6141,16 @@
       <c r="BB29" t="inlineStr"/>
       <c r="BC29" t="inlineStr"/>
       <c r="BD29" t="inlineStr"/>
+      <c r="BE29" t="inlineStr">
+        <is>
+          <t>92002_28</t>
+        </is>
+      </c>
+      <c r="BF29" t="inlineStr">
+        <is>
+          <t>028 ECOLE MATERNELLE VAL DE BIEVRE</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -6045,6 +6335,16 @@
       <c r="BB30" t="inlineStr"/>
       <c r="BC30" t="inlineStr"/>
       <c r="BD30" t="inlineStr"/>
+      <c r="BE30" t="inlineStr">
+        <is>
+          <t>92002_29</t>
+        </is>
+      </c>
+      <c r="BF30" t="inlineStr">
+        <is>
+          <t>029 ECOLE ELEM DU NOYER DORE REFECTOI</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -6229,6 +6529,16 @@
       <c r="BB31" t="inlineStr"/>
       <c r="BC31" t="inlineStr"/>
       <c r="BD31" t="inlineStr"/>
+      <c r="BE31" t="inlineStr">
+        <is>
+          <t>92002_30</t>
+        </is>
+      </c>
+      <c r="BF31" t="inlineStr">
+        <is>
+          <t>030 ECOLE MATERNELLE ANATOLE FRANCE</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -6413,6 +6723,16 @@
       <c r="BB32" t="inlineStr"/>
       <c r="BC32" t="inlineStr"/>
       <c r="BD32" t="inlineStr"/>
+      <c r="BE32" t="inlineStr">
+        <is>
+          <t>92002_31</t>
+        </is>
+      </c>
+      <c r="BF32" t="inlineStr">
+        <is>
+          <t>031 ECOLE ELEMENTAIRE ANATOLE FRANCE</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -6597,6 +6917,16 @@
       <c r="BB33" t="inlineStr"/>
       <c r="BC33" t="inlineStr"/>
       <c r="BD33" t="inlineStr"/>
+      <c r="BE33" t="inlineStr">
+        <is>
+          <t>92002_32</t>
+        </is>
+      </c>
+      <c r="BF33" t="inlineStr">
+        <is>
+          <t>032 CONSERVATOIRE DARIUS MILHAUD</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -6781,6 +7111,16 @@
       <c r="BB34" t="inlineStr"/>
       <c r="BC34" t="inlineStr"/>
       <c r="BD34" t="inlineStr"/>
+      <c r="BE34" t="inlineStr">
+        <is>
+          <t>92002_33</t>
+        </is>
+      </c>
+      <c r="BF34" t="inlineStr">
+        <is>
+          <t>033 ECOLE MATERNELLE DES RABATS</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -6965,6 +7305,16 @@
       <c r="BB35" t="inlineStr"/>
       <c r="BC35" t="inlineStr"/>
       <c r="BD35" t="inlineStr"/>
+      <c r="BE35" t="inlineStr">
+        <is>
+          <t>92002_34</t>
+        </is>
+      </c>
+      <c r="BF35" t="inlineStr">
+        <is>
+          <t>034 ECOLE MATERN DUNOYER DE SEGONZAC</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -7149,6 +7499,16 @@
       <c r="BB36" t="inlineStr"/>
       <c r="BC36" t="inlineStr"/>
       <c r="BD36" t="inlineStr"/>
+      <c r="BE36" t="inlineStr">
+        <is>
+          <t>92002_35</t>
+        </is>
+      </c>
+      <c r="BF36" t="inlineStr">
+        <is>
+          <t>035 ECOLE ELEM DUNOYER DE SEGONZAC</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -7333,6 +7693,16 @@
       <c r="BB37" t="inlineStr"/>
       <c r="BC37" t="inlineStr"/>
       <c r="BD37" t="inlineStr"/>
+      <c r="BE37" t="inlineStr">
+        <is>
+          <t>92002_36</t>
+        </is>
+      </c>
+      <c r="BF37" t="inlineStr">
+        <is>
+          <t>036 ECOLE MATERNELLE DES RABATS</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -7517,6 +7887,16 @@
       <c r="BB38" t="inlineStr"/>
       <c r="BC38" t="inlineStr"/>
       <c r="BD38" t="inlineStr"/>
+      <c r="BE38" t="inlineStr">
+        <is>
+          <t>92002_37</t>
+        </is>
+      </c>
+      <c r="BF38" t="inlineStr">
+        <is>
+          <t>037 CENTRE ANDRE MALRAUX</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -7701,6 +8081,16 @@
       <c r="BB39" t="inlineStr"/>
       <c r="BC39" t="inlineStr"/>
       <c r="BD39" t="inlineStr"/>
+      <c r="BE39" t="inlineStr">
+        <is>
+          <t>92002_38</t>
+        </is>
+      </c>
+      <c r="BF39" t="inlineStr">
+        <is>
+          <t>038 ECOLE ELEMENTAIRE ANDRE PASQUIER</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -7885,6 +8275,16 @@
       <c r="BB40" t="inlineStr"/>
       <c r="BC40" t="inlineStr"/>
       <c r="BD40" t="inlineStr"/>
+      <c r="BE40" t="inlineStr">
+        <is>
+          <t>92002_39</t>
+        </is>
+      </c>
+      <c r="BF40" t="inlineStr">
+        <is>
+          <t>039 ECOLE MATERNELLE NOYER DORE</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -8069,6 +8469,16 @@
       <c r="BB41" t="inlineStr"/>
       <c r="BC41" t="inlineStr"/>
       <c r="BD41" t="inlineStr"/>
+      <c r="BE41" t="inlineStr">
+        <is>
+          <t>92002_40</t>
+        </is>
+      </c>
+      <c r="BF41" t="inlineStr">
+        <is>
+          <t>040 ECOLE MATERNELLE CHENIER</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -8253,6 +8663,16 @@
       <c r="BB42" t="inlineStr"/>
       <c r="BC42" t="inlineStr"/>
       <c r="BD42" t="inlineStr"/>
+      <c r="BE42" t="inlineStr">
+        <is>
+          <t>92002_41</t>
+        </is>
+      </c>
+      <c r="BF42" t="inlineStr">
+        <is>
+          <t>041 ESPACE VASARELY CLUB</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -8437,6 +8857,16 @@
       <c r="BB43" t="inlineStr"/>
       <c r="BC43" t="inlineStr"/>
       <c r="BD43" t="inlineStr"/>
+      <c r="BE43" t="inlineStr">
+        <is>
+          <t>92002_42</t>
+        </is>
+      </c>
+      <c r="BF43" t="inlineStr">
+        <is>
+          <t>042 ECOLE ELEM PAUL BERT SALLE POLYVA</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -8621,6 +9051,16 @@
       <c r="BB44" t="inlineStr"/>
       <c r="BC44" t="inlineStr"/>
       <c r="BD44" t="inlineStr"/>
+      <c r="BE44" t="inlineStr">
+        <is>
+          <t>92002_43</t>
+        </is>
+      </c>
+      <c r="BF44" t="inlineStr">
+        <is>
+          <t>043 GYMNASE DES RABATS</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -8805,6 +9245,16 @@
       <c r="BB45" t="inlineStr"/>
       <c r="BC45" t="inlineStr"/>
       <c r="BD45" t="inlineStr"/>
+      <c r="BE45" t="inlineStr">
+        <is>
+          <t>92002_44</t>
+        </is>
+      </c>
+      <c r="BF45" t="inlineStr">
+        <is>
+          <t>044 GYMNASE DESCARTES</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -8989,6 +9439,16 @@
       <c r="BB46" t="inlineStr"/>
       <c r="BC46" t="inlineStr"/>
       <c r="BD46" t="inlineStr"/>
+      <c r="BE46" t="inlineStr">
+        <is>
+          <t>92014_1</t>
+        </is>
+      </c>
+      <c r="BF46" t="inlineStr">
+        <is>
+          <t>LES COLONNES</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -9173,6 +9633,16 @@
       <c r="BB47" t="inlineStr"/>
       <c r="BC47" t="inlineStr"/>
       <c r="BD47" t="inlineStr"/>
+      <c r="BE47" t="inlineStr">
+        <is>
+          <t>92014_2</t>
+        </is>
+      </c>
+      <c r="BF47" t="inlineStr">
+        <is>
+          <t>ESPACE JOSEPH KESSEL</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -9357,6 +9827,16 @@
       <c r="BB48" t="inlineStr"/>
       <c r="BC48" t="inlineStr"/>
       <c r="BD48" t="inlineStr"/>
+      <c r="BE48" t="inlineStr">
+        <is>
+          <t>92014_3</t>
+        </is>
+      </c>
+      <c r="BF48" t="inlineStr">
+        <is>
+          <t>LES COLONNES</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -9541,6 +10021,16 @@
       <c r="BB49" t="inlineStr"/>
       <c r="BC49" t="inlineStr"/>
       <c r="BD49" t="inlineStr"/>
+      <c r="BE49" t="inlineStr">
+        <is>
+          <t>92014_4</t>
+        </is>
+      </c>
+      <c r="BF49" t="inlineStr">
+        <is>
+          <t>L AGOREINE</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -9725,6 +10215,16 @@
       <c r="BB50" t="inlineStr"/>
       <c r="BC50" t="inlineStr"/>
       <c r="BD50" t="inlineStr"/>
+      <c r="BE50" t="inlineStr">
+        <is>
+          <t>92014_5</t>
+        </is>
+      </c>
+      <c r="BF50" t="inlineStr">
+        <is>
+          <t>ECOLE MATERNELLE BAS COQUARTS</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -9909,6 +10409,16 @@
       <c r="BB51" t="inlineStr"/>
       <c r="BC51" t="inlineStr"/>
       <c r="BD51" t="inlineStr"/>
+      <c r="BE51" t="inlineStr">
+        <is>
+          <t>92014_6</t>
+        </is>
+      </c>
+      <c r="BF51" t="inlineStr">
+        <is>
+          <t>ECOLE MATERNELLE FAIENCERIE</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -10093,6 +10603,16 @@
       <c r="BB52" t="inlineStr"/>
       <c r="BC52" t="inlineStr"/>
       <c r="BD52" t="inlineStr"/>
+      <c r="BE52" t="inlineStr">
+        <is>
+          <t>92014_7</t>
+        </is>
+      </c>
+      <c r="BF52" t="inlineStr">
+        <is>
+          <t>CENTRE DE LOISIRS MATERNEL</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -10277,6 +10797,16 @@
       <c r="BB53" t="inlineStr"/>
       <c r="BC53" t="inlineStr"/>
       <c r="BD53" t="inlineStr"/>
+      <c r="BE53" t="inlineStr">
+        <is>
+          <t>92014_8</t>
+        </is>
+      </c>
+      <c r="BF53" t="inlineStr">
+        <is>
+          <t>ECOLE PRIMAIRE FAIENCERIE</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -10461,6 +10991,16 @@
       <c r="BB54" t="inlineStr"/>
       <c r="BC54" t="inlineStr"/>
       <c r="BD54" t="inlineStr"/>
+      <c r="BE54" t="inlineStr">
+        <is>
+          <t>92014_9</t>
+        </is>
+      </c>
+      <c r="BF54" t="inlineStr">
+        <is>
+          <t>ECOLE PRIMAIRE FAIENCERIE</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -10645,6 +11185,16 @@
       <c r="BB55" t="inlineStr"/>
       <c r="BC55" t="inlineStr"/>
       <c r="BD55" t="inlineStr"/>
+      <c r="BE55" t="inlineStr">
+        <is>
+          <t>92014_10</t>
+        </is>
+      </c>
+      <c r="BF55" t="inlineStr">
+        <is>
+          <t>ECOLE PRIMAIRE REPUBLIQUE</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -10829,6 +11379,16 @@
       <c r="BB56" t="inlineStr"/>
       <c r="BC56" t="inlineStr"/>
       <c r="BD56" t="inlineStr"/>
+      <c r="BE56" t="inlineStr">
+        <is>
+          <t>92014_11</t>
+        </is>
+      </c>
+      <c r="BF56" t="inlineStr">
+        <is>
+          <t>RESIDENCE DE LA VALLEE</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -11013,6 +11573,16 @@
       <c r="BB57" t="inlineStr"/>
       <c r="BC57" t="inlineStr"/>
       <c r="BD57" t="inlineStr"/>
+      <c r="BE57" t="inlineStr">
+        <is>
+          <t>92014_12</t>
+        </is>
+      </c>
+      <c r="BF57" t="inlineStr">
+        <is>
+          <t>MATERNELLE FONTAINE GRELOT</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -11197,6 +11767,16 @@
       <c r="BB58" t="inlineStr"/>
       <c r="BC58" t="inlineStr"/>
       <c r="BD58" t="inlineStr"/>
+      <c r="BE58" t="inlineStr">
+        <is>
+          <t>92014_13</t>
+        </is>
+      </c>
+      <c r="BF58" t="inlineStr">
+        <is>
+          <t>MATERNELLE FONTAINE GRELOT</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -11381,6 +11961,16 @@
       <c r="BB59" t="inlineStr"/>
       <c r="BC59" t="inlineStr"/>
       <c r="BD59" t="inlineStr"/>
+      <c r="BE59" t="inlineStr">
+        <is>
+          <t>92014_14</t>
+        </is>
+      </c>
+      <c r="BF59" t="inlineStr">
+        <is>
+          <t>SALLE FRANCOISE DOLTO</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -11565,6 +12155,16 @@
       <c r="BB60" t="inlineStr"/>
       <c r="BC60" t="inlineStr"/>
       <c r="BD60" t="inlineStr"/>
+      <c r="BE60" t="inlineStr">
+        <is>
+          <t>92019_1</t>
+        </is>
+      </c>
+      <c r="BF60" t="inlineStr">
+        <is>
+          <t>HOTEL DE VILLE</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -11749,6 +12349,16 @@
       <c r="BB61" t="inlineStr"/>
       <c r="BC61" t="inlineStr"/>
       <c r="BD61" t="inlineStr"/>
+      <c r="BE61" t="inlineStr">
+        <is>
+          <t>92019_2</t>
+        </is>
+      </c>
+      <c r="BF61" t="inlineStr">
+        <is>
+          <t>ECOLE ELEMENTAIRE PIERRE BROSSOLETTE</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -11933,6 +12543,16 @@
       <c r="BB62" t="inlineStr"/>
       <c r="BC62" t="inlineStr"/>
       <c r="BD62" t="inlineStr"/>
+      <c r="BE62" t="inlineStr">
+        <is>
+          <t>92019_3</t>
+        </is>
+      </c>
+      <c r="BF62" t="inlineStr">
+        <is>
+          <t>GYMNASE PIERRE BROSSOLETTE</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -12117,6 +12737,16 @@
       <c r="BB63" t="inlineStr"/>
       <c r="BC63" t="inlineStr"/>
       <c r="BD63" t="inlineStr"/>
+      <c r="BE63" t="inlineStr">
+        <is>
+          <t>92019_4</t>
+        </is>
+      </c>
+      <c r="BF63" t="inlineStr">
+        <is>
+          <t>ECOLE MATERNELLE PIERRE BROSSOLETTE</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -12301,6 +12931,16 @@
       <c r="BB64" t="inlineStr"/>
       <c r="BC64" t="inlineStr"/>
       <c r="BD64" t="inlineStr"/>
+      <c r="BE64" t="inlineStr">
+        <is>
+          <t>92019_5</t>
+        </is>
+      </c>
+      <c r="BF64" t="inlineStr">
+        <is>
+          <t>ECOLE PIERRE MENDES FRANCE</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -12485,6 +13125,16 @@
       <c r="BB65" t="inlineStr"/>
       <c r="BC65" t="inlineStr"/>
       <c r="BD65" t="inlineStr"/>
+      <c r="BE65" t="inlineStr">
+        <is>
+          <t>92019_6</t>
+        </is>
+      </c>
+      <c r="BF65" t="inlineStr">
+        <is>
+          <t>ECOLE PIERRE MENDES FRANCE</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -12669,6 +13319,16 @@
       <c r="BB66" t="inlineStr"/>
       <c r="BC66" t="inlineStr"/>
       <c r="BD66" t="inlineStr"/>
+      <c r="BE66" t="inlineStr">
+        <is>
+          <t>92019_7</t>
+        </is>
+      </c>
+      <c r="BF66" t="inlineStr">
+        <is>
+          <t>ECOLE MATERNELLE THOMAS MASARYK</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -12853,6 +13513,16 @@
       <c r="BB67" t="inlineStr"/>
       <c r="BC67" t="inlineStr"/>
       <c r="BD67" t="inlineStr"/>
+      <c r="BE67" t="inlineStr">
+        <is>
+          <t>92019_8</t>
+        </is>
+      </c>
+      <c r="BF67" t="inlineStr">
+        <is>
+          <t>CRECHE MAGDELEINE RENDU</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -13037,6 +13707,16 @@
       <c r="BB68" t="inlineStr"/>
       <c r="BC68" t="inlineStr"/>
       <c r="BD68" t="inlineStr"/>
+      <c r="BE68" t="inlineStr">
+        <is>
+          <t>92019_9</t>
+        </is>
+      </c>
+      <c r="BF68" t="inlineStr">
+        <is>
+          <t>ECOLE LEONARD DE VINCI</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -13221,6 +13901,16 @@
       <c r="BB69" t="inlineStr"/>
       <c r="BC69" t="inlineStr"/>
       <c r="BD69" t="inlineStr"/>
+      <c r="BE69" t="inlineStr">
+        <is>
+          <t>92019_10</t>
+        </is>
+      </c>
+      <c r="BF69" t="inlineStr">
+        <is>
+          <t>ECOLE JEAN JAURES</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -13405,6 +14095,16 @@
       <c r="BB70" t="inlineStr"/>
       <c r="BC70" t="inlineStr"/>
       <c r="BD70" t="inlineStr"/>
+      <c r="BE70" t="inlineStr">
+        <is>
+          <t>92019_11</t>
+        </is>
+      </c>
+      <c r="BF70" t="inlineStr">
+        <is>
+          <t>ECOLE JEAN JAURES</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -13589,6 +14289,16 @@
       <c r="BB71" t="inlineStr"/>
       <c r="BC71" t="inlineStr"/>
       <c r="BD71" t="inlineStr"/>
+      <c r="BE71" t="inlineStr">
+        <is>
+          <t>92019_12</t>
+        </is>
+      </c>
+      <c r="BF71" t="inlineStr">
+        <is>
+          <t>ECOLE JULES VERNE</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -13773,6 +14483,16 @@
       <c r="BB72" t="inlineStr"/>
       <c r="BC72" t="inlineStr"/>
       <c r="BD72" t="inlineStr"/>
+      <c r="BE72" t="inlineStr">
+        <is>
+          <t>92019_13</t>
+        </is>
+      </c>
+      <c r="BF72" t="inlineStr">
+        <is>
+          <t>ECOLE JULES VERNE</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -13957,6 +14677,16 @@
       <c r="BB73" t="inlineStr"/>
       <c r="BC73" t="inlineStr"/>
       <c r="BD73" t="inlineStr"/>
+      <c r="BE73" t="inlineStr">
+        <is>
+          <t>92019_14</t>
+        </is>
+      </c>
+      <c r="BF73" t="inlineStr">
+        <is>
+          <t>ECOLE JULES VERNE</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -14141,6 +14871,16 @@
       <c r="BB74" t="inlineStr"/>
       <c r="BC74" t="inlineStr"/>
       <c r="BD74" t="inlineStr"/>
+      <c r="BE74" t="inlineStr">
+        <is>
+          <t>92019_15</t>
+        </is>
+      </c>
+      <c r="BF74" t="inlineStr">
+        <is>
+          <t>COLLEGE PIERRE BROSSOLETTE</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -14325,6 +15065,16 @@
       <c r="BB75" t="inlineStr"/>
       <c r="BC75" t="inlineStr"/>
       <c r="BD75" t="inlineStr"/>
+      <c r="BE75" t="inlineStr">
+        <is>
+          <t>92019_16</t>
+        </is>
+      </c>
+      <c r="BF75" t="inlineStr">
+        <is>
+          <t>ECOLE MATERNELLE DES MOUILLEBOEUFS</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -14509,6 +15259,16 @@
       <c r="BB76" t="inlineStr"/>
       <c r="BC76" t="inlineStr"/>
       <c r="BD76" t="inlineStr"/>
+      <c r="BE76" t="inlineStr">
+        <is>
+          <t>92019_17</t>
+        </is>
+      </c>
+      <c r="BF76" t="inlineStr">
+        <is>
+          <t>ECOLE PIERRE BROSSOLETTE MATERNELLE</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -14693,6 +15453,16 @@
       <c r="BB77" t="inlineStr"/>
       <c r="BC77" t="inlineStr"/>
       <c r="BD77" t="inlineStr"/>
+      <c r="BE77" t="inlineStr">
+        <is>
+          <t>92019_18</t>
+        </is>
+      </c>
+      <c r="BF77" t="inlineStr">
+        <is>
+          <t>CENTRE DE LOISIRS SUZANNE BUISSON</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -14877,6 +15647,16 @@
       <c r="BB78" t="inlineStr"/>
       <c r="BC78" t="inlineStr"/>
       <c r="BD78" t="inlineStr"/>
+      <c r="BE78" t="inlineStr">
+        <is>
+          <t>92019_19</t>
+        </is>
+      </c>
+      <c r="BF78" t="inlineStr">
+        <is>
+          <t>ECOLE PIERRE MENDES FRANCE</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -15061,6 +15841,12 @@
       <c r="BB79" t="inlineStr"/>
       <c r="BC79" t="inlineStr"/>
       <c r="BD79" t="inlineStr"/>
+      <c r="BE79" t="inlineStr">
+        <is>
+          <t>92019_20</t>
+        </is>
+      </c>
+      <c r="BF79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -15245,6 +16031,16 @@
       <c r="BB80" t="inlineStr"/>
       <c r="BC80" t="inlineStr"/>
       <c r="BD80" t="inlineStr"/>
+      <c r="BE80" t="inlineStr">
+        <is>
+          <t>92071_1</t>
+        </is>
+      </c>
+      <c r="BF80" t="inlineStr">
+        <is>
+          <t>HOTEL DE VILLE</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -15429,6 +16225,16 @@
       <c r="BB81" t="inlineStr"/>
       <c r="BC81" t="inlineStr"/>
       <c r="BD81" t="inlineStr"/>
+      <c r="BE81" t="inlineStr">
+        <is>
+          <t>92071_2</t>
+        </is>
+      </c>
+      <c r="BF81" t="inlineStr">
+        <is>
+          <t>ECOLE MATERNELLE DU CENTRE</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -15613,6 +16419,16 @@
       <c r="BB82" t="inlineStr"/>
       <c r="BC82" t="inlineStr"/>
       <c r="BD82" t="inlineStr"/>
+      <c r="BE82" t="inlineStr">
+        <is>
+          <t>92071_3</t>
+        </is>
+      </c>
+      <c r="BF82" t="inlineStr">
+        <is>
+          <t>ECOLE ELEMENTAIRE DU CENTRE</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -15797,6 +16613,16 @@
       <c r="BB83" t="inlineStr"/>
       <c r="BC83" t="inlineStr"/>
       <c r="BD83" t="inlineStr"/>
+      <c r="BE83" t="inlineStr">
+        <is>
+          <t>92071_4</t>
+        </is>
+      </c>
+      <c r="BF83" t="inlineStr">
+        <is>
+          <t>LOCAUX D ACTIVITES</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -15981,6 +16807,16 @@
       <c r="BB84" t="inlineStr"/>
       <c r="BC84" t="inlineStr"/>
       <c r="BD84" t="inlineStr"/>
+      <c r="BE84" t="inlineStr">
+        <is>
+          <t>92071_5</t>
+        </is>
+      </c>
+      <c r="BF84" t="inlineStr">
+        <is>
+          <t>ANCIENNE MAIRIE</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -16165,6 +17001,16 @@
       <c r="BB85" t="inlineStr"/>
       <c r="BC85" t="inlineStr"/>
       <c r="BD85" t="inlineStr"/>
+      <c r="BE85" t="inlineStr">
+        <is>
+          <t>92071_6</t>
+        </is>
+      </c>
+      <c r="BF85" t="inlineStr">
+        <is>
+          <t>HALLE DES BLAGIS</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -16349,6 +17195,16 @@
       <c r="BB86" t="inlineStr"/>
       <c r="BC86" t="inlineStr"/>
       <c r="BD86" t="inlineStr"/>
+      <c r="BE86" t="inlineStr">
+        <is>
+          <t>92071_7</t>
+        </is>
+      </c>
+      <c r="BF86" t="inlineStr">
+        <is>
+          <t>HALLE DES BLAGIS</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -16533,6 +17389,16 @@
       <c r="BB87" t="inlineStr"/>
       <c r="BC87" t="inlineStr"/>
       <c r="BD87" t="inlineStr"/>
+      <c r="BE87" t="inlineStr">
+        <is>
+          <t>92071_8</t>
+        </is>
+      </c>
+      <c r="BF87" t="inlineStr">
+        <is>
+          <t>ECOLE DU PETIT CHAMBORD</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -16717,6 +17583,16 @@
       <c r="BB88" t="inlineStr"/>
       <c r="BC88" t="inlineStr"/>
       <c r="BD88" t="inlineStr"/>
+      <c r="BE88" t="inlineStr">
+        <is>
+          <t>92071_9</t>
+        </is>
+      </c>
+      <c r="BF88" t="inlineStr">
+        <is>
+          <t>CENTRE MATERNEL DES CLOS ST MARCEL</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -16901,6 +17777,16 @@
       <c r="BB89" t="inlineStr"/>
       <c r="BC89" t="inlineStr"/>
       <c r="BD89" t="inlineStr"/>
+      <c r="BE89" t="inlineStr">
+        <is>
+          <t>92071_10</t>
+        </is>
+      </c>
+      <c r="BF89" t="inlineStr">
+        <is>
+          <t>LOCAUX D ACTIVITES</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -17085,6 +17971,16 @@
       <c r="BB90" t="inlineStr"/>
       <c r="BC90" t="inlineStr"/>
       <c r="BD90" t="inlineStr"/>
+      <c r="BE90" t="inlineStr">
+        <is>
+          <t>92071_11</t>
+        </is>
+      </c>
+      <c r="BF90" t="inlineStr">
+        <is>
+          <t>ANCIENNE MAIRIE</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -17269,6 +18165,16 @@
       <c r="BB91" t="inlineStr"/>
       <c r="BC91" t="inlineStr"/>
       <c r="BD91" t="inlineStr"/>
+      <c r="BE91" t="inlineStr">
+        <is>
+          <t>92071_12</t>
+        </is>
+      </c>
+      <c r="BF91" t="inlineStr">
+        <is>
+          <t>ECOLE DU PETIT CHAMBORD</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -17453,6 +18359,16 @@
       <c r="BB92" t="inlineStr"/>
       <c r="BC92" t="inlineStr"/>
       <c r="BD92" t="inlineStr"/>
+      <c r="BE92" t="inlineStr">
+        <is>
+          <t>92071_13</t>
+        </is>
+      </c>
+      <c r="BF92" t="inlineStr">
+        <is>
+          <t>ECOLE ELEMENTAIRE DES BLAGIS</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -17637,6 +18553,16 @@
       <c r="BB93" t="inlineStr"/>
       <c r="BC93" t="inlineStr"/>
       <c r="BD93" t="inlineStr"/>
+      <c r="BE93" t="inlineStr">
+        <is>
+          <t>92071_14</t>
+        </is>
+      </c>
+      <c r="BF93" t="inlineStr">
+        <is>
+          <t>ACCUEIL MATERNEL CLOS SAINT MARCEL</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>